<commit_message>
match data.xlsx and json properties
</commit_message>
<xml_diff>
--- a/fun/jemmekrowboy/src/camping_matt.xlsx
+++ b/fun/jemmekrowboy/src/camping_matt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,77 +11,86 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>model_name</t>
+  </si>
+  <si>
+    <t>img_link</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>r_value</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>pack_dimension</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
   <si>
     <t xml:space="preserve">Camp Mat Self Inflating - Isomatte
 </t>
   </si>
   <si>
-    <t>Trail Lite - Sleeping mat</t>
-  </si>
-  <si>
-    <t>Nemo Tensor Insulated</t>
-  </si>
-  <si>
-    <t>img_link</t>
-  </si>
-  <si>
     <t>https://www.bfgcdn.com/1500_1500_90/560-0478-0112/sea-to-summit-camp-mat-self-inflating-isomatte.jpg</t>
   </si>
   <si>
-    <t>https://www.bfgcdn.com/1500_1500_90/560-0571-0111/therm-a-rest-trail-lite-isomatte.jpg</t>
-  </si>
-  <si>
-    <t>https://www.bfgcdn.com/1500_1500_90/560-0704-0111/nemo-tensor-isomatte.jpg</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>r_value</t>
-  </si>
-  <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>pack_dimension</t>
-  </si>
-  <si>
     <t>20x34 cm</t>
-  </si>
-  <si>
-    <t>28x15 cm</t>
-  </si>
-  <si>
-    <t>24x8</t>
-  </si>
-  <si>
-    <t>brand</t>
   </si>
   <si>
     <t xml:space="preserve">SEA TO SUMMIT
 </t>
   </si>
   <si>
+    <t>Sea to Summit Camp Mat Self Inflating - Buy camping mat online | Berg-freunde.ch</t>
+  </si>
+  <si>
+    <t>foam</t>
+  </si>
+  <si>
+    <t>Trail Lite - Sleeping mat</t>
+  </si>
+  <si>
+    <t>https://www.bfgcdn.com/1500_1500_90/560-0571-0111/therm-a-rest-trail-lite-isomatte.jpg</t>
+  </si>
+  <si>
+    <t>28x15 cm</t>
+  </si>
+  <si>
     <t xml:space="preserve">THERM-A-REST </t>
   </si>
   <si>
+    <t>Buy Thermarest Trail Lite sleeping mat online | Berg-freunde.ch</t>
+  </si>
+  <si>
+    <t>Nemo Tensor Insulated</t>
+  </si>
+  <si>
+    <t>https://www.bfgcdn.com/1500_1500_90/560-0704-0111/nemo-tensor-isomatte.jpg</t>
+  </si>
+  <si>
+    <t>24x8</t>
+  </si>
+  <si>
     <t>Nemo</t>
   </si>
   <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>Sea to Summit Camp Mat Self Inflating - Buy camping mat online | Berg-freunde.ch</t>
-  </si>
-  <si>
-    <t>Buy Thermarest Trail Lite sleeping mat online | Berg-freunde.ch</t>
-  </si>
-  <si>
     <t>Nemo Tensor - Isomatte | Versandkostenfrei | Berg-freunde.ch</t>
+  </si>
+  <si>
+    <t>air</t>
   </si>
 </sst>
 </file>
@@ -344,6 +353,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="11.0"/>
+    <col customWidth="1" min="3" max="3" width="7.25"/>
+    <col customWidth="1" min="4" max="4" width="7.75"/>
+    <col customWidth="1" min="5" max="5" width="7.0"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -358,113 +373,117 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>84.5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1020.0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1">
-        <v>84.5</v>
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="1">
         <v>118.95</v>
       </c>
       <c r="D3" s="1">
-        <v>196.95</v>
+        <v>3.2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>780.0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1">
-        <v>4.0</v>
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="1">
-        <v>3.2</v>
+        <v>196.95</v>
       </c>
       <c r="D4" s="1">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1020.0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>780.0</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="E4" s="1">
         <v>470.0</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="C2"/>
-    <hyperlink r:id="rId3" ref="D2"/>
-    <hyperlink r:id="rId4" ref="B8"/>
-    <hyperlink r:id="rId5" ref="C8"/>
-    <hyperlink r:id="rId6" ref="D8"/>
+    <hyperlink r:id="rId2" ref="H2"/>
+    <hyperlink r:id="rId3" ref="B3"/>
+    <hyperlink r:id="rId4" ref="H3"/>
+    <hyperlink r:id="rId5" ref="B4"/>
+    <hyperlink r:id="rId6" ref="H4"/>
   </hyperlinks>
   <drawing r:id="rId7"/>
 </worksheet>

</xml_diff>